<commit_message>
Update directory contents to remove temp files
</commit_message>
<xml_diff>
--- a/Controller-Model-View-Mapping.xlsx
+++ b/Controller-Model-View-Mapping.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$2:$Q$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$2:$Q$14</definedName>
     <definedName name="DataRetrieval">Lists!$A$16:$A$19</definedName>
     <definedName name="Focus">Lists!$A$22:$A$24</definedName>
     <definedName name="Http">Lists!$A$12:$A$13</definedName>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="112">
   <si>
     <t>Controller</t>
   </si>
@@ -370,13 +370,7 @@
     <t>"/stylist/{id}/client/new"</t>
   </si>
   <si>
-    <t>"/stylist/{sid}/client/delete/{cid}"</t>
-  </si>
-  <si>
     <t>"/stylist/"+sid</t>
-  </si>
-  <si>
-    <t>"/stylist/{sid}/client/update/{cid}"</t>
   </si>
   <si>
     <t>"/stylist/{sid}/update"</t>
@@ -508,6 +502,18 @@
   </si>
   <si>
     <t>UpdateClientPost</t>
+  </si>
+  <si>
+    <t>"/stylist/{sid}/client/{cid}/delete"</t>
+  </si>
+  <si>
+    <t>"/stylist/{sid}/client/{cid}/update"</t>
+  </si>
+  <si>
+    <t>ClientsDeleteAll</t>
+  </si>
+  <si>
+    <t>"/stylist/clients/delete"</t>
   </si>
 </sst>
 </file>
@@ -567,7 +573,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -625,12 +631,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -703,7 +703,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -715,7 +715,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -743,58 +744,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1099,7 +1054,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB70"/>
+  <dimension ref="A1:AD71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozenSplit"/>
@@ -1118,49 +1073,49 @@
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="35.7109375" customWidth="1"/>
-    <col min="15" max="15" width="21.140625" customWidth="1"/>
-    <col min="16" max="16" width="27.5703125" customWidth="1"/>
+    <col min="11" max="11" width="35.7109375" customWidth="1"/>
+    <col min="12" max="12" width="27.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" customWidth="1"/>
     <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="18.75">
-      <c r="A1" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="16" t="s">
+      <c r="A1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="18" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="21"/>
     </row>
     <row r="2" spans="1:28">
-      <c r="A2" s="12"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
@@ -1183,22 +1138,22 @@
         <v>56</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>8</v>
@@ -1237,23 +1192,23 @@
         <v>44</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2"/>
+      <c r="O3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="Q3" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB3" t="s">
         <v>31</v>
@@ -1273,8 +1228,8 @@
       <c r="E4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>99</v>
+      <c r="F4" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>27</v>
@@ -1286,19 +1241,19 @@
         <v>26</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="M4" s="2"/>
-      <c r="N4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
       <c r="P4" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>49</v>
@@ -1337,22 +1292,22 @@
         <v>27</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="P5" s="2" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>45</v>
@@ -1362,7 +1317,7 @@
       </c>
     </row>
     <row r="6" spans="1:28">
-      <c r="A6" s="11"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1376,7 +1331,7 @@
         <v>58</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>59</v>
@@ -1391,25 +1346,25 @@
         <v>60</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="N6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>96</v>
-      </c>
       <c r="Q6" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB6" t="s">
         <v>39</v>
@@ -1430,7 +1385,7 @@
         <v>66</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>59</v>
@@ -1442,18 +1397,18 @@
         <v>26</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K7" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="P7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="Q7" s="2"/>
       <c r="AB7" t="s">
         <v>40</v>
@@ -1474,7 +1429,7 @@
         <v>69</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>59</v>
@@ -1488,23 +1443,23 @@
       <c r="J8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="AB8" t="s">
@@ -1512,7 +1467,7 @@
       </c>
     </row>
     <row r="9" spans="1:28">
-      <c r="A9" s="2"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1523,7 +1478,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>38</v>
@@ -1532,13 +1487,13 @@
         <v>67</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>52</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -1563,10 +1518,10 @@
         <v>14</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>67</v>
@@ -1580,23 +1535,23 @@
       <c r="J10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N10" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="P10" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="AB10" t="s">
@@ -1604,7 +1559,7 @@
       </c>
     </row>
     <row r="11" spans="1:28">
-      <c r="A11" s="21"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
@@ -1615,10 +1570,10 @@
         <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>67</v>
@@ -1635,59 +1590,36 @@
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:28">
-      <c r="A12" s="24"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>30</v>
-      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:28">
-      <c r="A13" s="2"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1695,61 +1627,91 @@
         <v>37</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28">
+      <c r="A14" s="8"/>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="AB13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="M14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="AB14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:28">
@@ -1771,7 +1733,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="AB15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:28">
@@ -1792,6 +1754,9 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
+      <c r="AB16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="17" spans="1:28">
       <c r="A17" s="2"/>
@@ -1811,9 +1776,6 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
-      <c r="AB17" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="18" spans="1:28">
       <c r="A18" s="2"/>
@@ -1833,8 +1795,8 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-      <c r="AB18" t="s">
-        <v>64</v>
+      <c r="AB18" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:28">
@@ -1856,7 +1818,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="AB19" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:28">
@@ -1877,6 +1839,9 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
+      <c r="AB20" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="1:28">
       <c r="A21" s="2"/>
@@ -1896,9 +1861,6 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="AB21" s="1" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="22" spans="1:28">
       <c r="A22" s="2"/>
@@ -1918,8 +1880,8 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
-      <c r="AB22" t="s">
-        <v>14</v>
+      <c r="AB22" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:28">
@@ -1941,7 +1903,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="AB23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:28">
@@ -1962,6 +1924,9 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
+      <c r="AB24" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" spans="1:28">
       <c r="A25" s="2"/>
@@ -1981,9 +1946,6 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
-      <c r="AB25" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="26" spans="1:28">
       <c r="A26" s="2"/>
@@ -2003,8 +1965,8 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-      <c r="AB26" t="s">
-        <v>18</v>
+      <c r="AB26" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:28">
@@ -2026,7 +1988,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="AB27" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:28">
@@ -2048,7 +2010,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="AB28" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:28">
@@ -2070,7 +2032,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="AB29" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:28">
@@ -2092,7 +2054,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="AB30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:28">
@@ -2114,7 +2076,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="AB31" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:28">
@@ -2135,6 +2097,9 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
+      <c r="AB32" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="33" spans="1:28">
       <c r="A33" s="2"/>
@@ -2154,9 +2119,6 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
-      <c r="AB33" s="1" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="34" spans="1:28">
       <c r="A34" s="2"/>
@@ -2176,8 +2138,8 @@
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
-      <c r="AB34" s="7" t="s">
-        <v>102</v>
+      <c r="AB34" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:28">
@@ -2198,8 +2160,8 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
-      <c r="AB35" s="10" t="s">
-        <v>95</v>
+      <c r="AB35" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:28">
@@ -2220,8 +2182,8 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
-      <c r="AB36" s="7" t="s">
-        <v>89</v>
+      <c r="AB36" s="10" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:28">
@@ -2243,7 +2205,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="AB37" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:28">
@@ -2265,7 +2227,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="AB38" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:28">
@@ -2286,8 +2248,8 @@
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
-      <c r="AB39" t="s">
-        <v>96</v>
+      <c r="AB39" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:28">
@@ -2309,7 +2271,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="AB40" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:28">
@@ -2330,189 +2292,207 @@
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
+      <c r="AB41" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="42" spans="1:28">
-      <c r="AB42" s="1" t="s">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+    </row>
+    <row r="43" spans="1:28">
+      <c r="AB43" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28">
-      <c r="AB43" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:28">
       <c r="AB44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:28">
       <c r="AB45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28">
+      <c r="AB46" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:28">
-      <c r="AB47" s="1" t="s">
+    <row r="48" spans="1:28">
+      <c r="AB48" s="1" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="1:28">
-      <c r="AB48" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="49" spans="28:28">
       <c r="AB49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="28:28">
+      <c r="AB50" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="28:28">
-      <c r="AB51" s="1" t="s">
+    <row r="52" spans="28:28">
+      <c r="AB52" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="28:28">
-      <c r="AB52" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="53" spans="28:28">
       <c r="AB53" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="28:28">
       <c r="AB54" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="28:28">
       <c r="AB55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="28:28">
       <c r="AB56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="28:28">
+      <c r="AB57" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="28:28">
-      <c r="AB58" s="1" t="s">
+    <row r="59" spans="28:28">
+      <c r="AB59" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="28:28">
-      <c r="AB59" t="s">
+    <row r="60" spans="28:28">
+      <c r="AB60" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="28:28">
-      <c r="AB61" s="1" t="s">
+    <row r="62" spans="28:28">
+      <c r="AB62" s="1" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="62" spans="28:28">
-      <c r="AB62" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="63" spans="28:28">
       <c r="AB63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="28:28">
       <c r="AB64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65" spans="28:28">
       <c r="AB65" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="28:28">
+      <c r="AB66" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="28:28">
-      <c r="AB67" s="1" t="s">
+    <row r="68" spans="28:28">
+      <c r="AB68" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="28:28">
-      <c r="AB68" t="s">
+    <row r="69" spans="28:28">
+      <c r="AB69" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="28:28">
-      <c r="AB70" s="3" t="s">
-        <v>84</v>
+    <row r="71" spans="28:28">
+      <c r="AB71" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D2:Q13">
-    <filterColumn colId="12"/>
+  <autoFilter ref="D2:Q14">
+    <filterColumn colId="7"/>
+    <filterColumn colId="8"/>
   </autoFilter>
   <mergeCells count="5">
+    <mergeCell ref="K1:Q1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="K1:Q1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:P41">
-    <cfRule type="expression" dxfId="5" priority="2">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q41">
-    <cfRule type="expression" dxfId="4" priority="1">
+  <conditionalFormatting sqref="B3:Q42">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="14">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from List or Enter a Value" sqref="M3:M41">
-      <formula1>$AB$18:$AB$19</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="L42">
+      <formula1>$AB$37:$AB$41</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from List or Enter a Value" sqref="B3:B41">
-      <formula1>$AB$43:$AB$45</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="L3:L41">
+      <formula1>$AB$35:$AB$41</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="D3:D41">
-      <formula1>$AB$22:$AB$23</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="K3:K42">
+      <formula1>$AB$69</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from List or Enter a Value" sqref="C3:C41">
-      <formula1>$AB$62:$AB$65</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from List or Enter a Value" sqref="O3:O42">
+      <formula1>$AB$19:$AB$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="I3:I41">
-      <formula1>$AB$48:$AB$49</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from List or Enter a Value" sqref="B3:B42">
+      <formula1>$AB$44:$AB$46</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from List or Enter a Value" sqref="H3:H8 H10:H41">
-      <formula1>$AB$26:$AB$30</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="D3:D42">
+      <formula1>$AB$23:$AB$24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="J3:J41">
-      <formula1>$AB$59</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from List or Enter a Value" sqref="C3:C42">
+      <formula1>$AB$63:$AB$66</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="K3:K41">
-      <formula1>$AB$3:$AB$15</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="I3:I42">
+      <formula1>$AB$49:$AB$50</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="G3:G41">
-      <formula1>$AB$52:$AB$56</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from List or Enter a Value" sqref="H3:H8 H10:H42">
+      <formula1>$AB$27:$AB$31</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="L3:L41"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="N3:N41">
-      <formula1>$AB$68</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="J3:J42">
+      <formula1>$AB$60</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="M3:M42">
+      <formula1>$AB$3:$AB$16</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="G3:G42">
+      <formula1>$AB$53:$AB$57</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="N3:N42"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="H9">
-      <formula1>$AB$26:$AB$31</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="P41">
-      <formula1>$AB$36:$AB$40</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Select from List or Enter a Value" sqref="P3:P40">
-      <formula1>$AB$34:$AB$40</formula1>
+      <formula1>$AB$27:$AB$32</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="AB70" r:id="rId1"/>
-    <hyperlink ref="N8" r:id="rId2"/>
-    <hyperlink ref="N10" r:id="rId3"/>
+    <hyperlink ref="AB71" r:id="rId1"/>
+    <hyperlink ref="K8" r:id="rId2"/>
+    <hyperlink ref="K10" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>